<commit_message>
Added r file used in analysis and price by location
</commit_message>
<xml_diff>
--- a/marketingsim_finance_tracking.xlsx
+++ b/marketingsim_finance_tracking.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88b641755305afe2/Documents/SFU/PT_MBA/BUS_556_Marketing_Management/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88b641755305afe2/Documents/SFU/PT_MBA/BUS_556_Marketing_Management/Simulation/Marketing Simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{3E10FB67-3359-40D9-81C1-DFE316B5C0C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C9376FE2-1033-4407-900C-753C8511287E}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{3E10FB67-3359-40D9-81C1-DFE316B5C0C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D5170B4E-854C-41D7-8420-A740908634FB}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3C09797F-9BCA-414E-B286-41D1467F60D5}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -151,10 +151,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -473,7 +473,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>

</xml_diff>